<commit_message>
fix well name: remove spaces, to uppercase.
</commit_message>
<xml_diff>
--- a/inst/extdata/oilfield_100w_raw_data.xlsx
+++ b/inst/extdata/oilfield_100w_raw_data.xlsx
@@ -5026,6 +5026,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0749E9E8-E96D-4C27-93E7-495AC34869B0}" name="tblProsper" displayName="tblProsper" ref="A1:AY101" totalsRowShown="0">
+  <autoFilter ref="A1:AY101" xr:uid="{F4BF5C14-9634-481A-B4E9-683A37230558}"/>
   <sortState ref="A2:AY101">
     <sortCondition ref="F1:F101"/>
   </sortState>
@@ -5385,9 +5386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F5E7DE-FFDA-440E-8FE6-8CF5EA77E166}">
   <dimension ref="A1:AY101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A32" sqref="A32"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>